<commit_message>
actualizacion bd y interfazes
</commit_message>
<xml_diff>
--- a/exports/reporte.xlsx
+++ b/exports/reporte.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,11 @@
           <t>Cantidad</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -450,16 +455,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>platanos</t>
+          <t>soda</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2500.0</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>48.0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -468,16 +478,481 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>zanahorias</t>
+          <t>chezels</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5600.0</t>
+          <t>901.0</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>30634.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Manzanas</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1200.0</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>30</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>36000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Peras</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1000.0</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>25000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Plátanos</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>800.0</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>40</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>32000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Naranjas</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>950.0</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>47500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1500.0</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>30000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Uvas</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1800.0</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>15</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>27000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sandía</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2000.0</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>20000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Melón</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1700.0</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>20400.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Duraznos</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1300.0</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>22</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>28600.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Frutillas</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2200.0</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>17600.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Limones</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>600.0</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>35</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>21000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mandarinas</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>900.0</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>40</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>36000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cerezas</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>15000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Piñas</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2500.0</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>7</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>17500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mangos</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1600.0</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>9</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>14400.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Papayas</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1400.0</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>11</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>15400.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Perones</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1200.0</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>13</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>15600.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ciruelas</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1800.0</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>14</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>25200.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Granadas</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2100.0</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>12600.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Arándanos</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2900.0</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>11600.0</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -491,7 +966,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +999,402 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>juan</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5693475</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>peñuelas</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>carlos</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>56936485067</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>almendrez</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>56934563489</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Peñuelas</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>María</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>56987654321</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>La Serena</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>56923456789</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Coquimbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ana</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>56912345678</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ovalle</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>56999887766</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Vicuña</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Lucía</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>56988776655</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Andacollo</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Felipe</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>56977665544</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Tongoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Sofía</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>56966554433</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Guanaqueros</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Martín</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>56955443322</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Illapel</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Camila</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>56944332211</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Los Vilos</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Andrés</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>56933221100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Monte Patria</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Valentina</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>56922110099</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Combarbalá</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Rodrigo</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>56911009988</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>La Higuera</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Fernanda</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>56900998877</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Pisco Elqui</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Javier</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>56998765432</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>La Serena</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Daniela</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>56987651234</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Coquimbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Cristóbal</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>56976542345</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Tongoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Isidora</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>56965433456</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Guanaqueros</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Sebastián</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>56954324567</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>La Serena</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Antonia</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>56943215678</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Coquimbo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>